<commit_message>
update lithium further analysis
</commit_message>
<xml_diff>
--- a/lithium_further_analysis.xlsx
+++ b/lithium_further_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Florence/Documents/CFA/Climate Risk (Certification)/Hard_Commodity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C4A271-49EA-D243-B266-2276F1831152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BB35A6-CA7A-6742-A9D6-E69AFFC36172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="760" windowWidth="34560" windowHeight="18480" xr2:uid="{7D89A806-8ACD-214D-9640-67BB26CECAB5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="18480" activeTab="1" xr2:uid="{7D89A806-8ACD-214D-9640-67BB26CECAB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Highlights" sheetId="3" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>2) Different Time Frame, All else equal</t>
   </si>
   <si>
-    <t>Copper Demand for key energy transition (kt)</t>
-  </si>
-  <si>
     <t>Original Data Source: IEA</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
       </rPr>
       <t>Under the NZE scenario highlighted by the IEA, lithium demand is projected to increase tenfold by 2050 compared to 2023. While this prediction is plausible based on current technology, it remains vulnerable to substitution risks from future hydrogen fuel cell vehicles. Diversifying investments into other renewable energy vehicle technologies is necessary for ensuring balanced preparation on both the supply and demand sides. Additionally, due to robust demand, the percentage change in growth rate from the longest (27 years) to the shortest (7 years) period is more evident for lithium than for copper, with the highest reduction reaching 60.57% for lithium and 54.45% for copper under the NZE scenario.</t>
     </r>
+  </si>
+  <si>
+    <t>Lithium Demand for key energy transition (kt)</t>
   </si>
 </sst>
 </file>
@@ -865,22 +865,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96007073-8C50-B14B-BD55-98E79DCC59AC}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L10"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCB0BEC-515F-4649-B26A-39F2DE131043}">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1034,14 +1034,14 @@
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
     <row r="3" spans="1:24" s="1" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="30">
         <f>D12/B12-1</f>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="18" spans="1:24" s="1" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="14"/>
       <c r="D18" s="14"/>
@@ -1634,7 +1634,7 @@
     </row>
     <row r="19" spans="1:24" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>36</v>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>36</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="22" spans="1:24" s="1" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="14"/>
       <c r="D22" s="14"/>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="23" spans="1:24" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>36</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>36</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="27" spans="1:24" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="30">
         <f>(D12/$B$12)-1</f>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="28" spans="1:24" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" s="26">
         <f>D5-$B$5</f>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" s="31">
         <f>ROUND((D12/$B$12)^(1/D28)-1,4)</f>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H30" s="32">
         <f>H29/D29-1</f>

</xml_diff>